<commit_message>
added new case for soroe 1950-2099 GCM4 2.6
</commit_message>
<xml_diff>
--- a/software/3D-CMCC-Forest-Model/input/DKSoroe/ISIMIP/Stand_data_Andreas_Ibrom.xlsx
+++ b/software/3D-CMCC-Forest-Model/input/DKSoroe/ISIMIP/Stand_data_Andreas_Ibrom.xlsx
@@ -4,15 +4,16 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="DBH_m" sheetId="1" r:id="rId1"/>
     <sheet name="tree height" sheetId="3" r:id="rId2"/>
     <sheet name="age" sheetId="2" r:id="rId3"/>
     <sheet name="tree number" sheetId="4" r:id="rId4"/>
-    <sheet name="1996" sheetId="5" r:id="rId5"/>
-    <sheet name="2001" sheetId="6" r:id="rId6"/>
+    <sheet name="1950" sheetId="7" r:id="rId5"/>
+    <sheet name="1996" sheetId="5" r:id="rId6"/>
+    <sheet name="2001" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="Soroe_age_1921_2010" localSheetId="2">age!$A$1:$CI$8</definedName>
@@ -402,7 +403,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="15">
   <si>
     <t>class_1</t>
   </si>
@@ -804,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:CI17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BN1" workbookViewId="0">
-      <selection activeCell="BZ11" sqref="BZ11:BZ17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5378,8 +5379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:CI8"/>
   <sheetViews>
-    <sheetView topLeftCell="BI1" workbookViewId="0">
-      <selection activeCell="BZ2" sqref="BZ2:BZ8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7501,8 +7502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:CI8"/>
   <sheetViews>
-    <sheetView topLeftCell="AI1" workbookViewId="0">
-      <selection activeCell="BZ2" sqref="BZ2:BZ8"/>
+    <sheetView topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AA2" sqref="AA2:AA8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9626,8 +9627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:CI8"/>
   <sheetViews>
-    <sheetView topLeftCell="BN1" workbookViewId="0">
-      <selection activeCell="BZ2" sqref="BZ2:BZ8"/>
+    <sheetView topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AA2" sqref="AA2:AA8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11749,7 +11750,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D11"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11770,100 +11771,100 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2">
-        <v>7.2959999999999994</v>
+        <v>4.7829999999999995</v>
       </c>
       <c r="B2">
-        <v>8.4706901523995803</v>
+        <v>2.0890124395277598</v>
       </c>
       <c r="C2">
-        <v>75</v>
+        <v>29</v>
       </c>
       <c r="D2">
-        <v>34.511148796016997</v>
+        <v>138.039870849458</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3">
-        <v>9.7736000000000001</v>
+        <v>3.2348000000000003</v>
       </c>
       <c r="B3">
-        <v>10.446306652554201</v>
+        <v>2.7335003179871999</v>
       </c>
       <c r="C3">
-        <v>75</v>
+        <v>29</v>
       </c>
       <c r="D3">
-        <v>72.473412471635697</v>
+        <v>289.88372878386201</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4">
-        <v>15.689</v>
+        <v>3.6350000000000002</v>
       </c>
       <c r="B4">
-        <v>17.712121451009299</v>
+        <v>5.76902186020373</v>
       </c>
       <c r="C4">
-        <v>75</v>
+        <v>29</v>
       </c>
       <c r="D4">
-        <v>32.785591356216102</v>
+        <v>131.13787730698499</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5">
-        <v>25.412153846153799</v>
+        <v>4.6647692307692301</v>
       </c>
       <c r="B5">
-        <v>24.6573566191224</v>
+        <v>10.390201453270199</v>
       </c>
       <c r="C5">
-        <v>75</v>
+        <v>29</v>
       </c>
       <c r="D5">
-        <v>74.198969911436507</v>
+        <v>296.78572232633502</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6">
-        <v>33.638909090909102</v>
+        <v>8.5336363636363597</v>
       </c>
       <c r="B6">
-        <v>27.074373310396901</v>
+        <v>12.670895230873599</v>
       </c>
       <c r="C6">
-        <v>75</v>
+        <v>29</v>
       </c>
       <c r="D6">
-        <v>132.86792286466499</v>
+        <v>531.45350277041405</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7">
-        <v>41.03</v>
+        <v>8.6534999999999993</v>
       </c>
       <c r="B7">
-        <v>26.1096335420937</v>
+        <v>11.4752878098558</v>
       </c>
       <c r="C7">
-        <v>75</v>
+        <v>29</v>
       </c>
       <c r="D7">
-        <v>29.334476476614402</v>
+        <v>117.333890222039</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8">
-        <v>42.786000000000001</v>
+        <v>4.3259999999999996</v>
       </c>
       <c r="B8">
-        <v>34.825752289435798</v>
+        <v>21.519251902355801</v>
       </c>
       <c r="C8">
-        <v>75</v>
+        <v>29</v>
       </c>
       <c r="D8">
-        <v>5.1766723194025497</v>
+        <v>20.7059806274187</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -11877,18 +11878,18 @@
     <row r="11" spans="1:4">
       <c r="A11">
         <f>((A2*D2)+(A3*D3)+(A4*D4)+(A5*D5)+(A6*D6)+(A7*D7)+(A8*D8))/(SUM(D2:D8))</f>
-        <v>24.268275182735803</v>
+        <v>5.9653808910546449</v>
       </c>
       <c r="B11">
         <f>((B2*D2)+(B3*D3)+(B4*D4)+(B5*D5)+(B6*D6)+(B7*D7)+(B8*D8))/(SUM(D2:D8))</f>
-        <v>20.986529849009813</v>
+        <v>8.8157191005990505</v>
       </c>
       <c r="C11">
-        <v>75</v>
+        <v>29</v>
       </c>
       <c r="D11">
         <f>SUM(D2:D8)</f>
-        <v>381.34819419598722</v>
+        <v>1525.3405728865118</v>
       </c>
     </row>
   </sheetData>
@@ -11901,7 +11902,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11921,6 +11922,158 @@
       </c>
     </row>
     <row r="2" spans="1:4">
+      <c r="A2">
+        <v>7.2959999999999994</v>
+      </c>
+      <c r="B2">
+        <v>8.4706901523995803</v>
+      </c>
+      <c r="C2">
+        <v>75</v>
+      </c>
+      <c r="D2">
+        <v>34.511148796016997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>9.7736000000000001</v>
+      </c>
+      <c r="B3">
+        <v>10.446306652554201</v>
+      </c>
+      <c r="C3">
+        <v>75</v>
+      </c>
+      <c r="D3">
+        <v>72.473412471635697</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>15.689</v>
+      </c>
+      <c r="B4">
+        <v>17.712121451009299</v>
+      </c>
+      <c r="C4">
+        <v>75</v>
+      </c>
+      <c r="D4">
+        <v>32.785591356216102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>25.412153846153799</v>
+      </c>
+      <c r="B5">
+        <v>24.6573566191224</v>
+      </c>
+      <c r="C5">
+        <v>75</v>
+      </c>
+      <c r="D5">
+        <v>74.198969911436507</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>33.638909090909102</v>
+      </c>
+      <c r="B6">
+        <v>27.074373310396901</v>
+      </c>
+      <c r="C6">
+        <v>75</v>
+      </c>
+      <c r="D6">
+        <v>132.86792286466499</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>41.03</v>
+      </c>
+      <c r="B7">
+        <v>26.1096335420937</v>
+      </c>
+      <c r="C7">
+        <v>75</v>
+      </c>
+      <c r="D7">
+        <v>29.334476476614402</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>42.786000000000001</v>
+      </c>
+      <c r="B8">
+        <v>34.825752289435798</v>
+      </c>
+      <c r="C8">
+        <v>75</v>
+      </c>
+      <c r="D8">
+        <v>5.1766723194025497</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <f>((A2*D2)+(A3*D3)+(A4*D4)+(A5*D5)+(A6*D6)+(A7*D7)+(A8*D8))/(SUM(D2:D8))</f>
+        <v>24.268275182735803</v>
+      </c>
+      <c r="B11">
+        <f>((B2*D2)+(B3*D3)+(B4*D4)+(B5*D5)+(B6*D6)+(B7*D7)+(B8*D8))/(SUM(D2:D8))</f>
+        <v>20.986529849009813</v>
+      </c>
+      <c r="C11">
+        <v>75</v>
+      </c>
+      <c r="D11">
+        <f>SUM(D2:D8)</f>
+        <v>381.34819419598722</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="2">
         <v>7.2959999999999994</v>
       </c>

</xml_diff>